<commit_message>
rename Spacecraft function + validate restriction + graficos gerais
</commit_message>
<xml_diff>
--- a/Execucoes Gerais/novo_final_GEOreal2PDS_vs_AGEOreal2PDS.xlsx
+++ b/Execucoes Gerais/novo_final_GEOreal2PDS_vs_AGEOreal2PDS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13335" windowHeight="12360" firstSheet="1" activeTab="5"/>
+    <workbookView windowWidth="14460" windowHeight="7860" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GRI" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="SCH" sheetId="4" r:id="rId4"/>
     <sheet name="ACK" sheetId="5" r:id="rId5"/>
     <sheet name="BEA" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="26">
   <si>
     <t>NFE</t>
   </si>
@@ -74,16 +75,40 @@
   <si>
     <t>Execution Time: 132 s</t>
   </si>
+  <si>
+    <t>TIMESAT</t>
+  </si>
+  <si>
+    <t>CropPhen</t>
+  </si>
+  <si>
+    <t>Phenofit</t>
+  </si>
+  <si>
+    <t>DATimes</t>
+  </si>
+  <si>
+    <t>Extrair métricas de 1 série temporal</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Extrair métricas de 1+ séries temporais</t>
+  </si>
+  <si>
+    <t>Extrair métricas de um stack de imagens</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -91,6 +116,20 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -102,54 +141,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,6 +157,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -171,11 +180,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -202,39 +225,41 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -247,7 +272,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,67 +440,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,103 +452,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,11 +481,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -476,26 +507,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,8 +532,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -543,109 +568,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -654,37 +700,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1530,7 +1555,7 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
+          <c:max val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2460,7 +2485,6 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="100000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3389,7 +3413,7 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="10"/>
+          <c:max val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3467,6 +3491,7 @@
         <c:crossAx val="357432052"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5244,7 +5269,7 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1000"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6173,7 +6198,7 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
+          <c:max val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6251,6 +6276,7 @@
         <c:crossAx val="357432052"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -9676,13 +9702,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9690,7 +9716,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="685800" y="7423150"/>
+        <a:off x="685800" y="7432675"/>
         <a:ext cx="4114800" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
@@ -11651,8 +11677,8 @@
   <sheetPr/>
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B40" sqref="B1:B40"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -12281,7 +12307,7 @@
   <sheetPr/>
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B40" sqref="B1:B40"/>
     </sheetView>
   </sheetViews>
@@ -12903,8 +12929,8 @@
   <sheetPr/>
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B1:B40"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -13516,7 +13542,7 @@
   <sheetPr/>
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B40" sqref="B1:B40"/>
     </sheetView>
   </sheetViews>
@@ -14129,8 +14155,8 @@
   <sheetPr/>
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B1:B40"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -14733,8 +14759,8 @@
   <sheetPr/>
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -15398,4 +15424,77 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A5:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7" outlineLevelCol="7"/>
+  <sheetData>
+    <row r="5" spans="5:8">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>